<commit_message>
update for this week's rides
</commit_message>
<xml_diff>
--- a/api_allocate_modular/outputs/excel/assignments_2025-10-02_21-07.xlsx
+++ b/api_allocate_modular/outputs/excel/assignments_2025-10-02_21-07.xlsx
@@ -508,7 +508,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="19" customWidth="1" min="10" max="10"/>
     <col width="21" customWidth="1" min="11" max="11"/>
@@ -537,12 +537,12 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
+          <t>Driver: Kaitlyn Kim</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
           <t>Driver: Josh Paik</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>Driver: Kaitlyn Kim</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
@@ -589,39 +589,39 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
+          <t>Ben Kim</t>
+        </is>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Gabriel Ni</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="inlineStr">
+        <is>
+          <t>Lindsey Ro</t>
+        </is>
+      </c>
+      <c r="F3" s="11" t="inlineStr">
+        <is>
+          <t>Jane Yoo</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
+        </is>
+      </c>
+      <c r="J3" s="13" t="inlineStr">
+        <is>
+          <t>Lunch 💛</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
           <t>Daniel Kuo</t>
         </is>
       </c>
-      <c r="D3" s="10" t="inlineStr">
-        <is>
-          <t>Lindsey Ro</t>
-        </is>
-      </c>
-      <c r="E3" s="11" t="inlineStr">
-        <is>
-          <t>Jane Yoo</t>
-        </is>
-      </c>
-      <c r="F3" s="10" t="inlineStr">
-        <is>
-          <t>Eugene Seo</t>
-        </is>
-      </c>
-      <c r="G3" s="12" t="inlineStr">
-        <is>
-          <t>Isabelle Li</t>
-        </is>
-      </c>
-      <c r="J3" s="13" t="inlineStr">
-        <is>
-          <t>Lunch 💛</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
       <c r="L3" s="11" t="inlineStr">
         <is>
           <t>Rebecca Lu</t>
@@ -629,7 +629,7 @@
       </c>
       <c r="M3" s="12" t="inlineStr">
         <is>
-          <t>Claire Doh</t>
+          <t>Joann Jung</t>
         </is>
       </c>
       <c r="N3" s="1" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>Ben Kim</t>
+          <t>Daniel Kuo</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -654,39 +654,39 @@
           <t>Zoe Li</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>Eugene Seo</t>
+        </is>
+      </c>
+      <c r="F4" s="11" t="inlineStr">
         <is>
           <t>Grace Sowon Park</t>
         </is>
       </c>
-      <c r="F4" s="10" t="inlineStr">
+      <c r="G4" s="12" t="inlineStr">
+        <is>
+          <t>Cara Lee</t>
+        </is>
+      </c>
+      <c r="J4" s="14" t="inlineStr">
+        <is>
+          <t>NLK 🧡 (Special 1)</t>
+        </is>
+      </c>
+      <c r="K4" s="10" t="inlineStr">
         <is>
           <t>Gabriel Ni</t>
         </is>
       </c>
-      <c r="G4" s="12" t="inlineStr">
-        <is>
-          <t>Joanna Wei</t>
-        </is>
-      </c>
-      <c r="J4" s="14" t="inlineStr">
-        <is>
-          <t>NLK 🧡 (Special 1)</t>
-        </is>
-      </c>
-      <c r="K4" s="10" t="inlineStr">
-        <is>
-          <t>Zoe Li</t>
-        </is>
-      </c>
       <c r="L4" s="11" t="inlineStr">
         <is>
-          <t>Jane Yoo</t>
+          <t>Grace Sowon Park</t>
         </is>
       </c>
       <c r="M4" s="12" t="inlineStr">
         <is>
-          <t>Isabelle Li</t>
+          <t>Sam Ko</t>
         </is>
       </c>
       <c r="N4" s="10" t="inlineStr">
@@ -708,24 +708,24 @@
       </c>
       <c r="D5" s="12" t="inlineStr">
         <is>
-          <t>Kyle Hwang</t>
-        </is>
-      </c>
-      <c r="E5" s="12" t="inlineStr">
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>helena song🐟</t>
+        </is>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>Joanna Wei</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
         <is>
           <t>Sehyun Jung</t>
         </is>
       </c>
-      <c r="F5" s="11" t="inlineStr">
-        <is>
-          <t>helena song🐟</t>
-        </is>
-      </c>
-      <c r="G5" s="12" t="inlineStr">
-        <is>
-          <t>Joel Shim</t>
-        </is>
-      </c>
       <c r="J5" s="14" t="inlineStr">
         <is>
           <t>Special 2</t>
@@ -733,17 +733,17 @@
       </c>
       <c r="K5" s="10" t="inlineStr">
         <is>
-          <t>Gabriel Ni</t>
+          <t>Zoe Li</t>
         </is>
       </c>
       <c r="L5" s="11" t="inlineStr">
         <is>
-          <t>Grace Sowon Park</t>
+          <t>Jane Yoo</t>
         </is>
       </c>
       <c r="M5" s="12" t="inlineStr">
         <is>
-          <t>Sam Ko</t>
+          <t>Cara Lee</t>
         </is>
       </c>
       <c r="N5" s="12" t="inlineStr">
@@ -755,7 +755,7 @@
     <row r="6">
       <c r="C6" s="12" t="inlineStr">
         <is>
-          <t>Cara Lee</t>
+          <t>Joann Jung</t>
         </is>
       </c>
       <c r="D6" s="12" t="inlineStr">
@@ -763,14 +763,14 @@
           <t>Claire Doh</t>
         </is>
       </c>
-      <c r="E6" s="12" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
+      <c r="F6" s="12" t="inlineStr">
+        <is>
+          <t>Isabelle Li</t>
         </is>
       </c>
       <c r="G6" s="12" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Joel Shim</t>
         </is>
       </c>
       <c r="K6" s="11" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="L6" s="12" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Isabelle Li</t>
         </is>
       </c>
       <c r="M6" s="12" t="inlineStr">
         <is>
-          <t>Cara Lee</t>
+          <t>Claire Doh</t>
         </is>
       </c>
     </row>
@@ -835,14 +835,14 @@
     <row r="12">
       <c r="M12" s="12" t="inlineStr">
         <is>
-          <t>Sehyun Jung — No valid driver</t>
+          <t>Joanna Wei — No valid driver</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="M13" s="12" t="inlineStr">
         <is>
-          <t>Joanna Wei — No valid driver</t>
+          <t>Sehyun Jung — No valid driver</t>
         </is>
       </c>
     </row>

</xml_diff>